<commit_message>
Add data for Lombardy
</commit_message>
<xml_diff>
--- a/data/google_mobility_report.xlsx
+++ b/data/google_mobility_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikew\Desktop\University\TilburgUniversity\Master\thesis_corona\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CC2C79-1693-401C-B7E3-E220D7E1F179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEF6CCF-8715-4FCE-916E-28E1D7BD9333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14556" yWindow="5580" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,158 @@
     <author>Mike Weltevrede</author>
   </authors>
   <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{ABED1B27-171E-4515-BF40-B8C911AFF1EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mike Weltevrede:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mobility trends for places like restaurants,
+cafes, shopping centers, theme parks,
+museums, libraries, and movie theaters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{6B184DEF-4A92-4B20-8A46-1D11F06F80B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mike Weltevrede:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mobility trends for places like grocery
+markets, food warehouses, farmers
+markets, specialty food shops, drug stores,
+and pharmacies.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{898E19F8-FAEB-420E-A1C4-D19A757C4ACA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mike Weltevrede:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mobility trends for places like national parks,
+public beaches, marinas, dog parks, plazas,
+and public gardens</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{350CA0D0-1800-4ECF-BA64-04C1C494B51D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mike Weltevrede:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mobility trends for places like public transport
+hubs such as subway, bus, and train stations.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{F0304C52-76FE-4061-A3B3-DEA23223C037}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mike Weltevrede:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mobility trends for places of work.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{98A28AA7-64DD-42A4-AB2E-D2477BC6058D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mike Weltevrede:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mobility trends for places of residence.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B18" authorId="0" shapeId="0" xr:uid="{F4DC9FBE-B94A-4588-A266-EF13D027E284}">
       <text>
         <r>
@@ -910,7 +1062,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I1048576"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,11 +1726,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF115D2-B505-448D-8FA8-1C02DC5956C4}">
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,6 +1954,9 @@
       <c r="A4" s="2">
         <v>43882</v>
       </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -1812,6 +1967,9 @@
       <c r="A6" s="2">
         <v>43884</v>
       </c>
+      <c r="K6">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -1863,82 +2021,91 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43895</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43896</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43897</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43898</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43899</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43900</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43901</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43902</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43903</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43904</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43905</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43906</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43907</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43908</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43909</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43910</v>
       </c>
@@ -2153,10 +2320,10 @@
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:V3"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2385,21 +2552,33 @@
       <c r="A5" s="2">
         <v>43883</v>
       </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43884</v>
       </c>
+      <c r="K6">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43885</v>
       </c>
+      <c r="K7">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43886</v>
       </c>
+      <c r="K8">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -2425,6 +2604,9 @@
       <c r="A13" s="2">
         <v>43891</v>
       </c>
+      <c r="K13">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
@@ -2440,83 +2622,95 @@
       <c r="A16" s="2">
         <v>43894</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43895</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43896</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43897</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43898</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43899</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43900</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43901</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43902</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43903</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43904</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43905</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43906</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43907</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43908</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43909</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43910</v>
       </c>
@@ -2525,6 +2719,9 @@
       <c r="A33" s="2">
         <v>43911</v>
       </c>
+      <c r="K33">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
@@ -2535,6 +2732,9 @@
       <c r="A35" s="2">
         <v>43913</v>
       </c>
+      <c r="K35">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
@@ -2545,6 +2745,9 @@
       <c r="A37" s="2">
         <v>43915</v>
       </c>
+      <c r="K37">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
@@ -2554,6 +2757,9 @@
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43917</v>
+      </c>
+      <c r="K39">
+        <v>0.6</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
@@ -2731,10 +2937,10 @@
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:V3"/>
+      <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2958,56 +3164,89 @@
       <c r="A4" s="2">
         <v>43882</v>
       </c>
+      <c r="K4">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43883</v>
       </c>
+      <c r="K5">
+        <v>1.4</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43884</v>
       </c>
+      <c r="K6">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43885</v>
       </c>
+      <c r="K7">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43886</v>
       </c>
+      <c r="K8">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43887</v>
       </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43888</v>
       </c>
+      <c r="K10">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43889</v>
       </c>
+      <c r="K11">
+        <v>1.35</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43890</v>
       </c>
+      <c r="K12">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43891</v>
       </c>
+      <c r="K13">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>43892</v>
       </c>
+      <c r="K14">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
@@ -3019,82 +3258,115 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43895</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43896</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43897</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43898</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43899</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43900</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43901</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43902</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43903</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43904</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43905</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43906</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43907</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43908</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43909</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43910</v>
       </c>
@@ -3103,6 +3375,9 @@
       <c r="A33" s="2">
         <v>43911</v>
       </c>
+      <c r="K33">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
@@ -3112,6 +3387,9 @@
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43913</v>
+      </c>
+      <c r="K35">
+        <v>0.2</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
@@ -4337,10 +4615,10 @@
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:V3"/>
+      <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4568,11 +4846,17 @@
       <c r="A6" s="2">
         <v>43884</v>
       </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43885</v>
       </c>
+      <c r="K7">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -4619,82 +4903,88 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43895</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43896</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43897</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43898</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43899</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43900</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43901</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43902</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43903</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43904</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43905</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43906</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43907</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43908</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43909</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43910</v>
       </c>
@@ -4732,6 +5022,9 @@
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43917</v>
+      </c>
+      <c r="K39">
+        <v>0.2</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
@@ -4953,11 +5246,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EE9D81-D4EC-43F2-868A-7C2FAC871707}">
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:V3"/>
+      <selection pane="bottomRight" activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5185,11 +5478,17 @@
       <c r="A6" s="2">
         <v>43884</v>
       </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43885</v>
       </c>
+      <c r="K7">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -5236,84 +5535,96 @@
         <v>43894</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43895</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43896</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43897</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43898</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43899</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43900</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43901</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43902</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43903</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43904</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43905</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43906</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43907</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43908</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43909</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43910</v>
+      </c>
+      <c r="K32">
+        <v>1.4</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
@@ -5325,11 +5636,17 @@
       <c r="A34" s="2">
         <v>43912</v>
       </c>
+      <c r="K34">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43913</v>
       </c>
+      <c r="K35">
+        <v>1.4</v>
+      </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
@@ -5349,6 +5666,9 @@
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43917</v>
+      </c>
+      <c r="K39">
+        <v>1.4</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">

</xml_diff>